<commit_message>
completed POTD till today
</commit_message>
<xml_diff>
--- a/Leet Code Ranking.xlsx
+++ b/Leet Code Ranking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20393"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F32D12-384E-4948-AA8C-C9F3E95ED5BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A243187-EDD8-4F45-9828-13326AA4B6FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -33,12 +33,21 @@
   <si>
     <t>No of Questions completed</t>
   </si>
+  <si>
+    <t>&lt;500000 Rank</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Achieved ranking below 5 lacs and Nov month daily challenge</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="43" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,16 +109,238 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -117,11 +348,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -133,6 +375,43 @@
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="32" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -155,13 +434,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8493A64-E31A-490C-AD2B-575D5CA2C205}" name="Table1" displayName="Table1" ref="A1:D30" totalsRowShown="0">
-  <autoFilter ref="A1:D30" xr:uid="{AFBA861B-729F-4B67-955B-5E07D3FD50F7}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8493A64-E31A-490C-AD2B-575D5CA2C205}" name="Table1" displayName="Table1" ref="A1:E91" totalsRowShown="0">
+  <autoFilter ref="A1:E91" xr:uid="{AFBA861B-729F-4B67-955B-5E07D3FD50F7}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{7E313A19-0152-4BF9-AEDA-C26E729D1363}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{0B0C036A-F079-4FCF-8C2D-8548F6B15C81}" name="Ranking"/>
     <tableColumn id="3" xr3:uid="{FD862E2D-1E83-4917-8310-7ACA1681CBB6}" name="Difference"/>
     <tableColumn id="4" xr3:uid="{DD711082-FBFD-4FD6-97A2-7B6C00FC038C}" name="No of Questions completed"/>
+    <tableColumn id="5" xr3:uid="{E639446E-7191-404B-98FD-A1DD8C58839E}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -430,22 +710,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:P91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84:C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -462,6 +746,9 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -512,7 +799,7 @@
         <v>1560264</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C18" si="0">B4-B5</f>
+        <f t="shared" ref="C5:C85" si="0">B4-B5</f>
         <v>59240</v>
       </c>
       <c r="D5">
@@ -548,9 +835,7 @@
       <c r="D7">
         <v>60</v>
       </c>
-      <c r="N7" s="9">
-        <v>1233411</v>
-      </c>
+      <c r="N7" s="9"/>
     </row>
     <row r="8" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -566,11 +851,9 @@
       <c r="D8">
         <v>61</v>
       </c>
-      <c r="K8" s="8">
-        <v>1244394</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>45575</v>
       </c>
@@ -584,8 +867,9 @@
       <c r="D9">
         <v>63</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>45576</v>
       </c>
@@ -599,6 +883,7 @@
       <c r="D10">
         <v>64</v>
       </c>
+      <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -627,8 +912,9 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="I12" s="11"/>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
@@ -645,12 +931,8 @@
       <c r="D13">
         <v>66</v>
       </c>
-      <c r="J13" s="6">
-        <v>1318241</v>
-      </c>
-      <c r="L13" s="4">
-        <v>1369787</v>
-      </c>
+      <c r="J13" s="6"/>
+      <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -666,9 +948,7 @@
       <c r="D14">
         <v>71</v>
       </c>
-      <c r="L14" s="5">
-        <v>1371960</v>
-      </c>
+      <c r="L14" s="5"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -714,9 +994,8 @@
       <c r="D17">
         <v>77</v>
       </c>
-      <c r="J17" s="10">
-        <v>1188664</v>
-      </c>
+      <c r="H17" s="17"/>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
@@ -738,63 +1017,1077 @@
       <c r="A19" s="1">
         <v>45585</v>
       </c>
+      <c r="B19">
+        <v>1189685</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>-1021</v>
+      </c>
+      <c r="D19">
+        <v>80</v>
+      </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45586</v>
       </c>
+      <c r="B20">
+        <v>1168955</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>20730</v>
+      </c>
+      <c r="D20">
+        <v>82</v>
+      </c>
     </row>
     <row r="21" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>45587</v>
       </c>
-      <c r="M21" s="7">
-        <v>1280209</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1148982</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>19973</v>
+      </c>
+      <c r="D21">
+        <v>84</v>
+      </c>
+      <c r="M21" s="7"/>
+    </row>
+    <row r="22" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>45588</v>
       </c>
+      <c r="B22">
+        <v>1150010</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>-1028</v>
+      </c>
+      <c r="D22">
+        <v>84</v>
+      </c>
+      <c r="I22" s="18"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45589</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>1047618</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>102392</v>
+      </c>
+      <c r="D23">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>45590</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>1007084</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>40534</v>
+      </c>
+      <c r="D24">
+        <v>99</v>
+      </c>
+      <c r="H24" s="16"/>
+    </row>
+    <row r="25" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>45591</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>990898</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>16186</v>
+      </c>
+      <c r="D25">
+        <v>102</v>
+      </c>
+      <c r="H25" s="21"/>
+      <c r="J25" s="22"/>
+    </row>
+    <row r="26" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>45592</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>952361</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>38537</v>
+      </c>
+      <c r="D26">
+        <v>107</v>
+      </c>
+      <c r="I26" s="14"/>
+    </row>
+    <row r="27" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>45593</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>945531</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>6830</v>
+      </c>
+      <c r="D27">
+        <v>108</v>
+      </c>
+      <c r="F27" s="19"/>
+    </row>
+    <row r="28" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>45594</v>
       </c>
+      <c r="B28">
+        <v>931677</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>13854</v>
+      </c>
+      <c r="D28">
+        <v>110</v>
+      </c>
+      <c r="G28" s="20"/>
+      <c r="H28" s="23"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45595</v>
       </c>
+      <c r="B29">
+        <v>917953</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>13724</v>
+      </c>
+      <c r="D29">
+        <v>112</v>
+      </c>
+      <c r="I29" s="15"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45596</v>
+      </c>
+      <c r="B30">
+        <v>897660</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>20293</v>
+      </c>
+      <c r="D30">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>45597</v>
+      </c>
+      <c r="B31">
+        <v>865166</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>32494</v>
+      </c>
+      <c r="D31">
+        <v>120</v>
+      </c>
+      <c r="I31" s="26"/>
+      <c r="J31" s="24"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>45598</v>
+      </c>
+      <c r="B32">
+        <v>822236</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>42930</v>
+      </c>
+      <c r="D32">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>45599</v>
+      </c>
+      <c r="B33">
+        <v>787810</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>34426</v>
+      </c>
+      <c r="D33">
+        <v>133</v>
+      </c>
+      <c r="J33" s="25"/>
+    </row>
+    <row r="34" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>45600</v>
+      </c>
+      <c r="B34">
+        <v>777144</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>10666</v>
+      </c>
+      <c r="D34">
+        <v>135</v>
+      </c>
+      <c r="J34" s="39"/>
+    </row>
+    <row r="35" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>45601</v>
+      </c>
+      <c r="B35">
+        <v>740627</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>36517</v>
+      </c>
+      <c r="D35">
+        <v>142</v>
+      </c>
+      <c r="J35" s="34"/>
+    </row>
+    <row r="36" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>45602</v>
+      </c>
+      <c r="B36">
+        <v>721223</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>19404</v>
+      </c>
+      <c r="D36">
+        <v>146</v>
+      </c>
+      <c r="J36" s="36"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>45603</v>
+      </c>
+      <c r="B37">
+        <v>697847</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>23376</v>
+      </c>
+      <c r="D37">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>45604</v>
+      </c>
+      <c r="B38">
+        <v>687547</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>10300</v>
+      </c>
+      <c r="D38">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>45605</v>
+      </c>
+      <c r="B39">
+        <v>678735</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>8812</v>
+      </c>
+      <c r="D39">
+        <v>156</v>
+      </c>
+      <c r="J39" s="27"/>
+    </row>
+    <row r="40" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>45606</v>
+      </c>
+      <c r="B40">
+        <v>670121</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>8614</v>
+      </c>
+      <c r="D40">
+        <v>157</v>
+      </c>
+      <c r="H40" s="28"/>
+      <c r="I40" s="28"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>45607</v>
+      </c>
+      <c r="B41">
+        <v>640508</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>29613</v>
+      </c>
+      <c r="D41">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>45608</v>
+      </c>
+      <c r="B42">
+        <v>632857</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>7651</v>
+      </c>
+      <c r="D42">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>45609</v>
+      </c>
+      <c r="B43">
+        <v>621086</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>11771</v>
+      </c>
+      <c r="D43">
+        <v>169</v>
+      </c>
+      <c r="J43" s="30"/>
+    </row>
+    <row r="44" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>45610</v>
+      </c>
+      <c r="B44">
+        <v>609989</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>11097</v>
+      </c>
+      <c r="D44">
+        <v>171</v>
+      </c>
+      <c r="J44" s="31"/>
+      <c r="L44" s="29"/>
+    </row>
+    <row r="45" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>45611</v>
+      </c>
+      <c r="B45">
+        <v>592048</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>17941</v>
+      </c>
+      <c r="D45">
+        <v>176</v>
+      </c>
+      <c r="I45" s="33"/>
+      <c r="J45" s="35"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>45612</v>
+      </c>
+      <c r="B46">
+        <v>574557</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>17491</v>
+      </c>
+      <c r="D46">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>45613</v>
+      </c>
+      <c r="B47">
+        <v>557835</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>16722</v>
+      </c>
+      <c r="D47">
+        <v>187</v>
+      </c>
+      <c r="I47" s="32"/>
+    </row>
+    <row r="48" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>45614</v>
+      </c>
+      <c r="B48">
+        <v>551711</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>6124</v>
+      </c>
+      <c r="D48">
+        <v>189</v>
+      </c>
+      <c r="I48" s="32"/>
+    </row>
+    <row r="49" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>45615</v>
+      </c>
+      <c r="B49">
+        <v>548909</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>2802</v>
+      </c>
+      <c r="D49">
+        <v>190</v>
+      </c>
+      <c r="I49" s="40"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>45616</v>
+      </c>
+      <c r="B50">
+        <v>542771</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>6138</v>
+      </c>
+      <c r="D50">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>45617</v>
+      </c>
+      <c r="B51">
+        <v>518668</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>24103</v>
+      </c>
+      <c r="D51">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>45618</v>
+      </c>
+      <c r="B52">
+        <v>512564</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>6104</v>
+      </c>
+      <c r="D52">
+        <v>202</v>
+      </c>
+      <c r="I52" s="37"/>
+    </row>
+    <row r="53" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>45619</v>
+      </c>
+      <c r="B53">
+        <v>509846</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>2718</v>
+      </c>
+      <c r="D53">
+        <v>203</v>
+      </c>
+      <c r="I53" s="38"/>
+    </row>
+    <row r="54" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>45620</v>
+      </c>
+      <c r="B54">
+        <v>507272</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>2574</v>
+      </c>
+      <c r="D54">
+        <v>204</v>
+      </c>
+      <c r="I54" s="41"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>45621</v>
+      </c>
+      <c r="B55">
+        <v>507593</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>-321</v>
+      </c>
+      <c r="D55">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>45622</v>
+      </c>
+      <c r="B56">
+        <v>493191</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>14402</v>
+      </c>
+      <c r="D56">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>45623</v>
+      </c>
+      <c r="B57">
+        <v>490645</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>2546</v>
+      </c>
+      <c r="D57">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>45624</v>
+      </c>
+      <c r="B58">
+        <v>482561</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>8084</v>
+      </c>
+      <c r="D58">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>45625</v>
+      </c>
+      <c r="B59">
+        <v>480130</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>2431</v>
+      </c>
+      <c r="D59">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>45626</v>
+      </c>
+      <c r="B60">
+        <v>474813</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>5317</v>
+      </c>
+      <c r="D60">
+        <v>216</v>
+      </c>
+      <c r="E60" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="F60" s="43">
+        <v>250</v>
+      </c>
+      <c r="G60" s="44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>45627</v>
+      </c>
+      <c r="B61">
+        <v>467125</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>7688</v>
+      </c>
+      <c r="D61">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>45628</v>
+      </c>
+      <c r="B62">
+        <v>467499</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>-374</v>
+      </c>
+      <c r="D62">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>45629</v>
+      </c>
+      <c r="B63">
+        <v>457270</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>10229</v>
+      </c>
+      <c r="D63">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>45630</v>
+      </c>
+      <c r="B64">
+        <v>450081</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>7189</v>
+      </c>
+      <c r="D64">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>45631</v>
+      </c>
+      <c r="B65">
+        <v>447795</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>2286</v>
+      </c>
+      <c r="D65">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A66" s="1">
+        <v>45632</v>
+      </c>
+      <c r="B66">
+        <v>433409</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>14386</v>
+      </c>
+      <c r="D66">
+        <v>233</v>
+      </c>
+      <c r="G66" s="45"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>45633</v>
+      </c>
+      <c r="B67">
+        <v>431313</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="0"/>
+        <v>2096</v>
+      </c>
+      <c r="D67">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>45634</v>
+      </c>
+      <c r="B68">
+        <v>431625</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="0"/>
+        <v>-312</v>
+      </c>
+      <c r="D68">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>45635</v>
+      </c>
+      <c r="B69">
+        <v>427050</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="0"/>
+        <v>4575</v>
+      </c>
+      <c r="D69">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>45636</v>
+      </c>
+      <c r="B70">
+        <v>422552</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="0"/>
+        <v>4498</v>
+      </c>
+      <c r="D70">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>45637</v>
+      </c>
+      <c r="B71">
+        <v>420522</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="0"/>
+        <v>2030</v>
+      </c>
+      <c r="D71">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>45638</v>
+      </c>
+      <c r="B72">
+        <v>418559</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="0"/>
+        <v>1963</v>
+      </c>
+      <c r="D72">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>45639</v>
+      </c>
+      <c r="B73">
+        <v>416586</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="0"/>
+        <v>1973</v>
+      </c>
+      <c r="D73">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>45640</v>
+      </c>
+      <c r="B74">
+        <v>416818</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="0"/>
+        <v>-232</v>
+      </c>
+      <c r="D74">
+        <v>241</v>
+      </c>
+      <c r="G74" s="46"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>45641</v>
+      </c>
+      <c r="B75">
+        <v>414878</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="0"/>
+        <v>1940</v>
+      </c>
+      <c r="D75">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>45642</v>
+      </c>
+      <c r="B76">
+        <v>408370</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="0"/>
+        <v>6508</v>
+      </c>
+      <c r="D76">
+        <v>245</v>
+      </c>
+      <c r="G76" s="47"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>45643</v>
+      </c>
+      <c r="B77">
+        <v>406461</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="0"/>
+        <v>1909</v>
+      </c>
+      <c r="D77">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>45644</v>
+      </c>
+      <c r="B78">
+        <v>400377</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="0"/>
+        <v>6084</v>
+      </c>
+      <c r="D78">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>45645</v>
+      </c>
+      <c r="B79">
+        <v>400655</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="0"/>
+        <v>-278</v>
+      </c>
+      <c r="D79">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>45646</v>
+      </c>
+      <c r="B80">
+        <v>394484</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="0"/>
+        <v>6171</v>
+      </c>
+      <c r="D80">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>45647</v>
+      </c>
+      <c r="B81">
+        <v>392606</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="0"/>
+        <v>1878</v>
+      </c>
+      <c r="D81">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>45648</v>
+      </c>
+      <c r="B82">
+        <v>390838</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="0"/>
+        <v>1768</v>
+      </c>
+      <c r="D82">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>45649</v>
+      </c>
+      <c r="B83">
+        <v>385034</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="0"/>
+        <v>5804</v>
+      </c>
+      <c r="D83">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>45650</v>
+      </c>
+      <c r="B84">
+        <v>379255</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="0"/>
+        <v>5779</v>
+      </c>
+      <c r="D84">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>45651</v>
+      </c>
+      <c r="B85">
+        <v>371630</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="0"/>
+        <v>7625</v>
+      </c>
+      <c r="D85">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>45652</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>45653</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>45654</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>45655</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>45656</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>45657</v>
       </c>
     </row>
   </sheetData>

</xml_diff>